<commit_message>
changed graphs a bit
</commit_message>
<xml_diff>
--- a/Results/Graphs.xlsx
+++ b/Results/Graphs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-520" yWindow="460" windowWidth="29280" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="28720" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -126,76 +126,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="Roboto" charset="0"/>
-                <a:ea typeface="Roboto" charset="0"/>
-                <a:cs typeface="Roboto" charset="0"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" sz="1600"/>
-              <a:t>Percent</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="zh-CN" sz="1600"/>
-              <a:t> </a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" sz="1600"/>
-              <a:t>of Questions Answered</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" sz="1600" baseline="0"/>
-              <a:t> Correctly</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US" sz="1600"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="Roboto" charset="0"/>
-              <a:ea typeface="Roboto" charset="0"/>
-              <a:cs typeface="Roboto" charset="0"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -451,11 +382,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2091475152"/>
-        <c:axId val="-2091908768"/>
+        <c:axId val="-2070617184"/>
+        <c:axId val="-2088269280"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2091475152"/>
+        <c:axId val="-2070617184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -561,7 +492,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2091908768"/>
+        <c:crossAx val="-2088269280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -569,7 +500,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2091908768"/>
+        <c:axId val="-2088269280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -683,7 +614,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2091475152"/>
+        <c:crossAx val="-2070617184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -782,63 +713,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="Roboto" charset="0"/>
-                <a:ea typeface="Roboto" charset="0"/>
-                <a:cs typeface="Roboto" charset="0"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" sz="1600"/>
-              <a:t>Questions Answered by Difficulty</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="Roboto" charset="0"/>
-              <a:ea typeface="Roboto" charset="0"/>
-              <a:cs typeface="Roboto" charset="0"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -1094,11 +969,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2027417392"/>
-        <c:axId val="-2027420592"/>
+        <c:axId val="-2069420864"/>
+        <c:axId val="-2090269008"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2027417392"/>
+        <c:axId val="-2069420864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1201,7 +1076,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2027420592"/>
+        <c:crossAx val="-2090269008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1209,7 +1084,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2027420592"/>
+        <c:axId val="-2090269008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1250,7 +1125,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" sz="1200"/>
-                  <a:t>Questions Answered Correctly</a:t>
+                  <a:t>Total Corret</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1315,7 +1190,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2027417392"/>
+        <c:crossAx val="-2069420864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1414,63 +1289,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="Roboto" charset="0"/>
-                <a:ea typeface="Roboto" charset="0"/>
-                <a:cs typeface="Roboto" charset="0"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" sz="1600"/>
-              <a:t>Percent Questions Answered by Difficulty</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="Roboto" charset="0"/>
-              <a:ea typeface="Roboto" charset="0"/>
-              <a:cs typeface="Roboto" charset="0"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -1726,11 +1545,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2029997600"/>
-        <c:axId val="-2027510352"/>
+        <c:axId val="-2067335744"/>
+        <c:axId val="-2067329888"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2029997600"/>
+        <c:axId val="-2067335744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1828,7 +1647,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2027510352"/>
+        <c:crossAx val="-2067329888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1836,7 +1655,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2027510352"/>
+        <c:axId val="-2067329888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -1878,7 +1697,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" sz="1200"/>
-                  <a:t>Percent Questions  Answered</a:t>
+                  <a:t>Percent Correct</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1943,7 +1762,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2029997600"/>
+        <c:crossAx val="-2067335744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4017,8 +3836,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="E58" sqref="E58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>